<commit_message>
Updated BOM for this year.
</commit_message>
<xml_diff>
--- a/fab/SEM-Karifa-2022-BOM_JLCSMT.xlsx
+++ b/fab/SEM-Karifa-2022-BOM_JLCSMT.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20391"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hekk_Elek\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Github\SEM-Karifa2022\fab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F117AA0-35AD-4441-A1D3-C0D760D472E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -52,9 +51,6 @@
     <t>L1, L2, L3</t>
   </si>
   <si>
-    <t>C223341</t>
-  </si>
-  <si>
     <t>1mH</t>
   </si>
   <si>
@@ -94,9 +90,6 @@
     <t>RGB LED</t>
   </si>
   <si>
-    <t>C409779</t>
-  </si>
-  <si>
     <t>3528(mm)</t>
   </si>
   <si>
@@ -140,12 +133,18 @@
   </si>
   <si>
     <t>C21190</t>
+  </si>
+  <si>
+    <t>C223217</t>
+  </si>
+  <si>
+    <t>C2827321</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -604,23 +603,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="19.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="26" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="36.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.95" customHeight="1">
+    <row r="1" spans="1:8" ht="19.899999999999999" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -631,12 +630,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F1" s="10"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="19.95" customHeight="1">
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -653,9 +652,9 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="19.95" customHeight="1">
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>9</v>
@@ -664,141 +663,143 @@
         <v>1008</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>10</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E3"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="19.95" customHeight="1">
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="19.95" customHeight="1">
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="19.95" customHeight="1">
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E6"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="19.95" customHeight="1">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="19.95" customHeight="1">
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="19.95" customHeight="1">
+    <row r="9" spans="1:8" ht="19.899999999999999" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="19.95" customHeight="1">
+    <row r="10" spans="1:8" ht="19.899999999999999" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="19.95" customHeight="1">
+    <row r="11" spans="1:8" ht="19.899999999999999" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>

</xml_diff>